<commit_message>
50% completion of activities
</commit_message>
<xml_diff>
--- a/Apps formula (KB).xlsx
+++ b/Apps formula (KB).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="7547" windowHeight="2543" activeTab="5"/>
+    <workbookView windowWidth="22103" windowHeight="9935" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="User interface" sheetId="5" r:id="rId1"/>
@@ -535,11 +535,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -590,7 +590,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -598,29 +613,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -634,8 +626,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -664,19 +657,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -688,8 +681,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -698,6 +706,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -718,21 +733,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <i/>
       <sz val="11"/>
@@ -742,12 +742,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <name val="Tahoma"/>
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <name val="Tahoma"/>
       <charset val="134"/>
@@ -780,7 +780,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -792,43 +852,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -840,37 +894,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -882,43 +918,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -936,19 +936,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1111,24 +1111,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1157,6 +1144,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1180,25 +1191,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1210,130 +1210,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1347,7 +1347,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="177" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2432,7 +2432,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -2618,8 +2618,8 @@
   <sheetPr/>
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -2930,7 +2930,7 @@
   <sheetPr/>
   <dimension ref="B2:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>